<commit_message>
feture encypt and decrypt config
</commit_message>
<xml_diff>
--- a/iam/input_user_data.xlsx
+++ b/iam/input_user_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookairm3/Documents/Store Project/4ManFashion/iam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D822CE2-C3D0-FD49-8217-B93DE03A9F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CCF29F-0FB3-0D4C-B394-99DD579EC785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="24960" windowHeight="17120" xr2:uid="{16A8EC16-21B4-A944-86DB-D01CF581F036}"/>
   </bookViews>
@@ -36,51 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>dob</t>
-  </si>
-  <si>
-    <t>street</t>
-  </si>
-  <si>
-    <t>ward</t>
-  </si>
-  <si>
-    <t>district</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>Đạt</t>
-  </si>
-  <si>
-    <t>Phan</t>
-  </si>
-  <si>
-    <t>Đường Ok</t>
-  </si>
-  <si>
-    <t>Tam Thuấn</t>
-  </si>
-  <si>
-    <t>Phúc Thọ</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
   </si>
   <si>
     <t>password</t>
@@ -169,7 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -177,13 +138,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -527,105 +482,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD479A5-20EB-DD47-9215-AD9937D57F0F}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="18.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+    <row r="1" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
+    </row>
+    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="5">
-        <v>36572</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{A8DE6FBD-E1F1-494B-B7E1-146C8B9A71B3}"/>

</xml_diff>